<commit_message>
above 50 no upstream 1 file
</commit_message>
<xml_diff>
--- a/output/0/tRNA-Ala-TGC-3-2.xlsx
+++ b/output/0/tRNA-Ala-TGC-3-2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="59">
   <si>
     <t>chr12</t>
   </si>
@@ -189,99 +189,6 @@
   </si>
   <si>
     <t>36</t>
-  </si>
-  <si>
-    <t>125406440</t>
-  </si>
-  <si>
-    <t>125406463</t>
-  </si>
-  <si>
-    <t>125406443</t>
-  </si>
-  <si>
-    <t>80,80,80</t>
-  </si>
-  <si>
-    <t>AAAAATAAAAATGAAACACG</t>
-  </si>
-  <si>
-    <t>TGG</t>
-  </si>
-  <si>
-    <t>95% (67)</t>
-  </si>
-  <si>
-    <t>8% (20)</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>MIT Spec. Score: 0, Doench 2016: 95%, Moreno-Mateos: 8%</t>
-  </si>
-  <si>
-    <t>125406579</t>
-  </si>
-  <si>
-    <t>125406602</t>
-  </si>
-  <si>
-    <t>125406582</t>
-  </si>
-  <si>
-    <t>AGAAATGATACATGTTTGAA</t>
-  </si>
-  <si>
-    <t>22% (31)</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>125406813</t>
-  </si>
-  <si>
-    <t>125406836</t>
-  </si>
-  <si>
-    <t>125406816</t>
-  </si>
-  <si>
-    <t>TGCATGATCTCACTCACGTG</t>
-  </si>
-  <si>
-    <t>97% (69)</t>
-  </si>
-  <si>
-    <t>72% (56)</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>125406835</t>
-  </si>
-  <si>
-    <t>125406858</t>
-  </si>
-  <si>
-    <t>125406855</t>
-  </si>
-  <si>
-    <t>AGTATTTATCTTTCTGTGCC</t>
-  </si>
-  <si>
-    <t>59% (53)</t>
-  </si>
-  <si>
-    <t>13% (25)</t>
-  </si>
-  <si>
-    <t>71</t>
   </si>
 </sst>
 </file>
@@ -326,7 +233,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -745,242 +652,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" t="s">
-        <v>62</v>
-      </c>
-      <c r="I8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L8" t="s">
-        <v>64</v>
-      </c>
-      <c r="M8" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" t="s">
-        <v>65</v>
-      </c>
-      <c r="O8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P8" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>40</v>
-      </c>
-      <c r="R8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" t="s">
-        <v>72</v>
-      </c>
-      <c r="L9" t="s">
-        <v>20</v>
-      </c>
-      <c r="M9" t="s">
-        <v>10</v>
-      </c>
-      <c r="N9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" t="s">
-        <v>73</v>
-      </c>
-      <c r="P9" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>14</v>
-      </c>
-      <c r="R9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" t="s">
-        <v>78</v>
-      </c>
-      <c r="L10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M10" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" t="s">
-        <v>79</v>
-      </c>
-      <c r="O10" t="s">
-        <v>80</v>
-      </c>
-      <c r="P10" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>82</v>
-      </c>
-      <c r="R10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" t="s">
-        <v>86</v>
-      </c>
-      <c r="L11" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" t="s">
-        <v>87</v>
-      </c>
-      <c r="O11" t="s">
-        <v>88</v>
-      </c>
-      <c r="P11" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>89</v>
-      </c>
-      <c r="R11" t="s">
-        <v>15</v>
-      </c>
-      <c r="S11" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>